<commit_message>
PX-13 - Mapeamento de entidades
</commit_message>
<xml_diff>
--- a/src/main/resources/excel_formatado.xlsx
+++ b/src/main/resources/excel_formatado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FATEC\2024\2ºS\API_DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FATEC\2024\2ºS\API\POC_IA\llm\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{630F6A91-F9CE-4204-B818-5C8571FC776C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BE228D-1B7E-465C-9619-81BB69735CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{602C6D60-F8DD-41B2-A56B-D7C880C69657}"/>
+    <workbookView xWindow="-20610" yWindow="555" windowWidth="20730" windowHeight="11040" xr2:uid="{602C6D60-F8DD-41B2-A56B-D7C880C69657}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
   <si>
     <t>Tipo de Ação Seletiva</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Ana Pereira</t>
   </si>
   <si>
-    <t>Reprovado</t>
-  </si>
-  <si>
     <t>Precisa melhorar comunicação</t>
   </si>
   <si>
@@ -244,16 +241,31 @@
   </si>
   <si>
     <t>Alisson</t>
+  </si>
+  <si>
+    <t>8000.00</t>
+  </si>
+  <si>
+    <t>Excelente didatica</t>
+  </si>
+  <si>
+    <t>Matias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -292,6 +304,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0433DCF4-A650-4DFA-8B4B-A1E7FFE78CC1}">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -692,14 +707,14 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:28" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3">
         <v>45545.583333333336</v>
@@ -774,14 +789,14 @@
         <v>45560</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3">
         <v>45546.416666666664</v>
@@ -805,19 +820,19 @@
         <v>43</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="N3" s="4">
         <v>45540</v>
@@ -829,25 +844,25 @@
         <v>38</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="V3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="X3" s="4">
         <v>45529</v>
@@ -856,14 +871,14 @@
         <v>45565</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
     <row r="4" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3">
         <v>45550.625</v>
@@ -872,7 +887,7 @@
         <v>45560</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>26</v>
@@ -884,22 +899,22 @@
         <v>45548</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="N4" s="4">
         <v>45537</v>
@@ -908,28 +923,28 @@
         <v>45563</v>
       </c>
       <c r="P4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="V4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="X4" s="4">
         <v>45536</v>
@@ -938,12 +953,93 @@
         <v>45566</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
+    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45546.625</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45553</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45557</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45548</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="4">
+        <v>45537</v>
+      </c>
+      <c r="O5" s="4">
+        <v>45563</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X5" s="4">
+        <v>45536</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>45566</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>